<commit_message>
Master table updated with correct sorption, isotherm plots also updated. Still need to update SCM results.
</commit_message>
<xml_diff>
--- a/Manuscript/Figures/Data/Figure5b-GOE Tetradentate Data.xlsx
+++ b/Manuscript/Figures/Data/Figure5b-GOE Tetradentate Data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Dropbox (Personal)\work\MIT Graduate Work\Research\RadiumSorption\Manuscript\Figures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Dropbox (Personal)\work\MIT Graduate Work\Research\RadiumSorption\Manuscript\Figures\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -363,7 +363,7 @@
   <dimension ref="A1:F82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:F1"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -696,10 +696,10 @@
         <v>-5.6532399999999997E-4</v>
       </c>
       <c r="C17">
-        <v>0.88256124174599648</v>
+        <v>0.94362105126578921</v>
       </c>
       <c r="D17">
-        <v>1.2380080330185188E-2</v>
+        <v>5.9433182421027844E-3</v>
       </c>
       <c r="E17">
         <v>8.99</v>
@@ -716,10 +716,10 @@
         <v>-5.5345399999999999E-4</v>
       </c>
       <c r="C18">
-        <v>0.86500040865270356</v>
+        <v>0.93519060357189066</v>
       </c>
       <c r="D18">
-        <v>2.0938721162594591E-2</v>
+        <v>1.0052073987640393E-2</v>
       </c>
       <c r="E18">
         <v>9</v>
@@ -736,10 +736,10 @@
         <v>-5.3516700000000002E-4</v>
       </c>
       <c r="C19">
-        <v>0.7947515905100685</v>
+        <v>0.90146617923715444</v>
       </c>
       <c r="D19">
-        <v>3.1727197811657781E-2</v>
+        <v>1.5231309369218682E-2</v>
       </c>
       <c r="E19">
         <v>9.0066666666666659</v>
@@ -756,10 +756,10 @@
         <v>-5.0738900000000002E-4</v>
       </c>
       <c r="C20">
-        <v>0.79252023684441408</v>
+        <v>0.9003949709257405</v>
       </c>
       <c r="D20">
-        <v>1.2130001255289546E-2</v>
+        <v>5.8232625164407106E-3</v>
       </c>
       <c r="E20">
         <v>9.0033333333333321</v>

</xml_diff>

<commit_message>
Numerical values and data updated for new stock calculations, now need to update figures.
</commit_message>
<xml_diff>
--- a/Manuscript/Figures/Data/Figure5b-GOE Tetradentate Data.xlsx
+++ b/Manuscript/Figures/Data/Figure5b-GOE Tetradentate Data.xlsx
@@ -363,7 +363,7 @@
   <dimension ref="A1:F82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -393,7 +393,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>-5.8477599999999996E-4</v>
+        <v>-5.8477646057199999E-4</v>
       </c>
       <c r="C2">
         <v>-0.32691797465356276</v>
@@ -413,7 +413,7 @@
         <v>2.1</v>
       </c>
       <c r="B3">
-        <v>-5.8477099999999999E-4</v>
+        <v>-5.8477142137400003E-4</v>
       </c>
       <c r="C3">
         <v>-6.6058113074162358E-2</v>
@@ -433,7 +433,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B4">
-        <v>-5.8476700000000003E-4</v>
+        <v>-5.8476679864299995E-4</v>
       </c>
       <c r="C4">
         <v>-5.6853056739888524E-2</v>
@@ -453,7 +453,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="B5">
-        <v>-5.8476100000000005E-4</v>
+        <v>-5.8476063208000003E-4</v>
       </c>
       <c r="C5">
         <v>-3.0755110980200395E-2</v>
@@ -473,7 +473,7 @@
         <v>2.4</v>
       </c>
       <c r="B6">
-        <v>-5.8474899999999997E-4</v>
+        <v>-5.8474932247400005E-4</v>
       </c>
       <c r="C6">
         <v>-3.2080914497226588E-2</v>
@@ -493,7 +493,7 @@
         <v>2.5</v>
       </c>
       <c r="B7">
-        <v>-5.8472600000000004E-4</v>
+        <v>-5.8472605153099999E-4</v>
       </c>
       <c r="C7">
         <v>-0.16377890535858927</v>
@@ -513,7 +513,7 @@
         <v>2.6</v>
       </c>
       <c r="B8">
-        <v>-5.8467800000000004E-4</v>
+        <v>-5.8467810525300004E-4</v>
       </c>
       <c r="C8">
         <v>5.704467214633905E-2</v>
@@ -533,7 +533,7 @@
         <v>2.7</v>
       </c>
       <c r="B9">
-        <v>-5.8458299999999996E-4</v>
+        <v>-5.8458251305200002E-4</v>
       </c>
       <c r="C9">
         <v>2.0545505008660991E-3</v>
@@ -553,7 +553,7 @@
         <v>2.8</v>
       </c>
       <c r="B10">
-        <v>-5.8439899999999999E-4</v>
+        <v>-5.8439916722700003E-4</v>
       </c>
       <c r="C10">
         <v>9.2316558212439045E-2</v>
@@ -573,7 +573,7 @@
         <v>2.9</v>
       </c>
       <c r="B11">
-        <v>-5.8406099999999998E-4</v>
+        <v>-5.8406019795899996E-4</v>
       </c>
       <c r="C11">
         <v>7.5122390800120495E-2</v>
@@ -593,7 +593,7 @@
         <v>3</v>
       </c>
       <c r="B12">
-        <v>-5.8345599999999999E-4</v>
+        <v>-5.8345445943599995E-4</v>
       </c>
       <c r="C12">
         <v>6.1140495675667011E-2</v>
@@ -613,7 +613,7 @@
         <v>3.1</v>
       </c>
       <c r="B13">
-        <v>-5.8240400000000002E-4</v>
+        <v>-5.8240100784400005E-4</v>
       </c>
       <c r="C13">
         <v>0.18288226450296075</v>
@@ -633,7 +633,7 @@
         <v>3.2</v>
       </c>
       <c r="B14">
-        <v>-5.8062499999999998E-4</v>
+        <v>-5.8061776242600001E-4</v>
       </c>
       <c r="C14">
         <v>0.1335388156980645</v>
@@ -653,7 +653,7 @@
         <v>3.3</v>
       </c>
       <c r="B15">
-        <v>-5.7768100000000003E-4</v>
+        <v>-5.7766749215699997E-4</v>
       </c>
       <c r="C15">
         <v>0.17736857395780428</v>
@@ -673,7 +673,7 @@
         <v>3.4</v>
       </c>
       <c r="B16">
-        <v>-5.7291099999999995E-4</v>
+        <v>-5.7288529583599999E-4</v>
       </c>
       <c r="C16">
         <v>0.14380761898517525</v>
@@ -693,7 +693,7 @@
         <v>3.5</v>
       </c>
       <c r="B17">
-        <v>-5.6532399999999997E-4</v>
+        <v>-5.6527500260199995E-4</v>
       </c>
       <c r="C17">
         <v>0.94362105126578921</v>
@@ -713,7 +713,7 @@
         <v>3.6</v>
       </c>
       <c r="B18">
-        <v>-5.5345399999999999E-4</v>
+        <v>-5.5336448200599998E-4</v>
       </c>
       <c r="C18">
         <v>0.93519060357189066</v>
@@ -733,7 +733,7 @@
         <v>3.7</v>
       </c>
       <c r="B19">
-        <v>-5.3516700000000002E-4</v>
+        <v>-5.3500606705400003E-4</v>
       </c>
       <c r="C19">
         <v>0.90146617923715444</v>
@@ -753,7 +753,7 @@
         <v>3.8</v>
       </c>
       <c r="B20">
-        <v>-5.0738900000000002E-4</v>
+        <v>-5.0710485226299995E-4</v>
       </c>
       <c r="C20">
         <v>0.9003949709257405</v>
@@ -773,7 +773,7 @@
         <v>3.9</v>
       </c>
       <c r="B21">
-        <v>-4.6574700000000003E-4</v>
+        <v>-4.6525402617699998E-4</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -781,7 +781,7 @@
         <v>4</v>
       </c>
       <c r="B22">
-        <v>-4.0409400000000002E-4</v>
+        <v>-4.0325316161000002E-4</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -789,7 +789,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="B23">
-        <v>-3.1389800000000001E-4</v>
+        <v>-3.1248347782600002E-4</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -797,7 +797,7 @@
         <v>4.2</v>
       </c>
       <c r="B24">
-        <v>-1.8346500000000001E-4</v>
+        <v>-1.8111509638000001E-4</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -805,7 +805,7 @@
         <v>4.3</v>
       </c>
       <c r="B25" s="1">
-        <v>3.0199999999999999E-6</v>
+        <v>6.8723226201199997E-6</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -813,7 +813,7 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="B26">
-        <v>2.6660200000000001E-4</v>
+        <v>2.7285898286200002E-4</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -821,7 +821,7 @@
         <v>4.5</v>
       </c>
       <c r="B27">
-        <v>6.3487899999999998E-4</v>
+        <v>6.4491927966899996E-4</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -829,7 +829,7 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="B28">
-        <v>1.143308E-3</v>
+        <v>1.15924894859E-3</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -837,7 +837,7 @@
         <v>4.7</v>
       </c>
       <c r="B29">
-        <v>1.836493E-3</v>
+        <v>1.8615429855999999E-3</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -845,7 +845,7 @@
         <v>4.8</v>
       </c>
       <c r="B30">
-        <v>2.7691230000000001E-3</v>
+        <v>2.8080881075E-3</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -853,7 +853,7 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="B31">
-        <v>4.0062250000000004E-3</v>
+        <v>4.0662213893400004E-3</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -861,7 +861,7 @@
         <v>5</v>
       </c>
       <c r="B32">
-        <v>5.6222679999999997E-3</v>
+        <v>5.7136965936499997E-3</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -869,7 +869,7 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="B33">
-        <v>7.6985680000000003E-3</v>
+        <v>7.8364316155299998E-3</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -877,7 +877,7 @@
         <v>5.2</v>
       </c>
       <c r="B34">
-        <v>1.0318518E-2</v>
+        <v>1.0524147136799999E-2</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -885,7 +885,7 @@
         <v>5.3</v>
       </c>
       <c r="B35">
-        <v>1.3560361999999999E-2</v>
+        <v>1.3863625862699999E-2</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -893,7 +893,7 @@
         <v>5.4</v>
       </c>
       <c r="B36">
-        <v>1.748773E-2</v>
+        <v>1.7929788093900001E-2</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -901,7 +901,7 @@
         <v>5.5</v>
       </c>
       <c r="B37">
-        <v>2.2138846E-2</v>
+        <v>2.2775496357800001E-2</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -909,7 +909,7 @@
         <v>5.6</v>
       </c>
       <c r="B38">
-        <v>2.7516210999999999E-2</v>
+        <v>2.8421847812099998E-2</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -917,7 +917,7 @@
         <v>5.7</v>
       </c>
       <c r="B39">
-        <v>3.3579179000000001E-2</v>
+        <v>3.4851412099699997E-2</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -925,7 +925,7 @@
         <v>5.8</v>
       </c>
       <c r="B40">
-        <v>4.0242053999999999E-2</v>
+        <v>4.2007041730500003E-2</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -933,7 +933,7 @@
         <v>5.9</v>
       </c>
       <c r="B41">
-        <v>4.7379578999999998E-2</v>
+        <v>4.9798200749299998E-2</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -941,7 +941,7 @@
         <v>6</v>
       </c>
       <c r="B42">
-        <v>5.4840123999999997E-2</v>
+        <v>5.8115198723E-2</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -949,7 +949,7 @@
         <v>6.1</v>
       </c>
       <c r="B43">
-        <v>6.2464849000000003E-2</v>
+        <v>6.6849697721499998E-2</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -957,7 +957,7 @@
         <v>6.2</v>
       </c>
       <c r="B44">
-        <v>7.0109446000000006E-2</v>
+        <v>7.5918138324000004E-2</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -965,7 +965,7 @@
         <v>6.3</v>
       </c>
       <c r="B45">
-        <v>7.7664422999999996E-2</v>
+        <v>8.5284036308499997E-2</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -973,7 +973,7 @@
         <v>6.4</v>
       </c>
       <c r="B46">
-        <v>8.5070617000000001E-2</v>
+        <v>9.4975710433500005E-2</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -981,7 +981,7 @@
         <v>6.5</v>
       </c>
       <c r="B47">
-        <v>9.2328269000000004E-2</v>
+        <v>0.105097564273</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -989,7 +989,7 @@
         <v>6.6</v>
       </c>
       <c r="B48">
-        <v>9.9499958999999999E-2</v>
+        <v>0.115834801369</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -997,7 +997,7 @@
         <v>6.7</v>
       </c>
       <c r="B49">
-        <v>0.106709049</v>
+        <v>0.127452664203</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -1005,7 +1005,7 @@
         <v>6.8</v>
       </c>
       <c r="B50">
-        <v>0.114135875</v>
+        <v>0.14029157624999999</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -1013,7 +1013,7 @@
         <v>6.9</v>
       </c>
       <c r="B51">
-        <v>0.122013676</v>
+        <v>0.154758984307</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -1021,7 +1021,7 @@
         <v>7</v>
       </c>
       <c r="B52">
-        <v>0.13062549400000001</v>
+        <v>0.17131757577500001</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -1029,7 +1029,7 @@
         <v>7.1</v>
       </c>
       <c r="B53">
-        <v>0.14030234</v>
+        <v>0.19046830073500001</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -1037,7 +1037,7 @@
         <v>7.2</v>
       </c>
       <c r="B54">
-        <v>0.15142201</v>
+        <v>0.21272566936599999</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -1045,7 +1045,7 @@
         <v>7.3</v>
       </c>
       <c r="B55">
-        <v>0.16440711299999999</v>
+        <v>0.23858252425900001</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -1053,7 +1053,7 @@
         <v>7.4</v>
       </c>
       <c r="B56">
-        <v>0.17972011900000001</v>
+        <v>0.26846234310900002</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -1061,7 +1061,7 @@
         <v>7.5</v>
       </c>
       <c r="B57">
-        <v>0.19785265499999999</v>
+        <v>0.30265952501400001</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -1069,7 +1069,7 @@
         <v>7.6</v>
       </c>
       <c r="B58">
-        <v>0.21930588600000001</v>
+        <v>0.34127222674000002</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -1077,7 +1077,7 @@
         <v>7.7</v>
       </c>
       <c r="B59">
-        <v>0.244558894</v>
+        <v>0.384137591793</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -1085,7 +1085,7 @@
         <v>7.8</v>
       </c>
       <c r="B60">
-        <v>0.27402330800000002</v>
+        <v>0.430784590099</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -1093,15 +1093,15 @@
         <v>7.9</v>
       </c>
       <c r="B61">
-        <v>0.30798403600000002</v>
+        <v>0.48042065554199997</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>8</v>
+        <v>7.9999999999</v>
       </c>
       <c r="B62">
-        <v>0.34653140500000001</v>
+        <v>0.53196644757900002</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -1109,7 +1109,7 @@
         <v>8.1</v>
       </c>
       <c r="B63">
-        <v>0.389494114</v>
+        <v>0.58414121044099998</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -1117,7 +1117,7 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="B64">
-        <v>0.43638840099999998</v>
+        <v>0.63558776122899996</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -1125,7 +1125,7 @@
         <v>8.3000000000000007</v>
       </c>
       <c r="B65">
-        <v>0.48640102499999999</v>
+        <v>0.68501290854800001</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -1133,7 +1133,7 @@
         <v>8.4</v>
       </c>
       <c r="B66">
-        <v>0.53842056999999999</v>
+        <v>0.73131377720599999</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -1141,7 +1141,7 @@
         <v>8.5</v>
       </c>
       <c r="B67">
-        <v>0.59112162999999995</v>
+        <v>0.77366544613199995</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
@@ -1149,7 +1149,7 @@
         <v>8.6</v>
       </c>
       <c r="B68">
-        <v>0.64309170900000001</v>
+        <v>0.81155802083999995</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -1157,7 +1157,7 @@
         <v>8.6999999999999993</v>
       </c>
       <c r="B69">
-        <v>0.69297694499999996</v>
+        <v>0.844785735752</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -1165,7 +1165,7 @@
         <v>8.8000000000000007</v>
       </c>
       <c r="B70">
-        <v>0.73961617999999996</v>
+        <v>0.87340116331999995</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
@@ -1173,7 +1173,7 @@
         <v>8.9</v>
       </c>
       <c r="B71">
-        <v>0.78213696399999999</v>
+        <v>0.89765150550999995</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
@@ -1181,15 +1181,15 @@
         <v>9</v>
       </c>
       <c r="B72">
-        <v>0.81999951299999996</v>
+        <v>0.91791211648500004</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>9.1</v>
+        <v>9.0999999997999996</v>
       </c>
       <c r="B73">
-        <v>0.85298960899999998</v>
+        <v>0.93462753358100004</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
@@ -1197,7 +1197,7 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="B74">
-        <v>0.88117285300000003</v>
+        <v>0.948265015268</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
@@ -1205,7 +1205,7 @@
         <v>9.3000000000000007</v>
       </c>
       <c r="B75">
-        <v>0.90482755100000001</v>
+        <v>0.95928149768600002</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
@@ -1213,7 +1213,7 @@
         <v>9.4</v>
       </c>
       <c r="B76">
-        <v>0.92437243199999997</v>
+        <v>0.96810245692300001</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
@@ -1221,7 +1221,7 @@
         <v>9.5</v>
       </c>
       <c r="B77">
-        <v>0.94030086999999996</v>
+        <v>0.97511016721099997</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
@@ -1229,7 +1229,7 @@
         <v>9.6</v>
       </c>
       <c r="B78">
-        <v>0.95312795100000003</v>
+        <v>0.98063877047000003</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -1237,7 +1237,7 @@
         <v>9.6999999999999993</v>
       </c>
       <c r="B79">
-        <v>0.96335233799999997</v>
+        <v>0.98497394685100004</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
@@ -1245,7 +1245,7 @@
         <v>9.8000000000000007</v>
       </c>
       <c r="B80">
-        <v>0.97143196399999998</v>
+        <v>0.98835547923400002</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
@@ -1253,7 +1253,7 @@
         <v>9.9</v>
       </c>
       <c r="B81">
-        <v>0.97777108800000001</v>
+        <v>0.99098147154399996</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
@@ -1261,7 +1261,7 @@
         <v>10</v>
       </c>
       <c r="B82">
-        <v>0.98271580000000003</v>
+        <v>0.99301335446799999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>